<commit_message>
add xlsx file download option
</commit_message>
<xml_diff>
--- a/backend/income_data.xlsx
+++ b/backend/income_data.xlsx
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,13 +398,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>source</v>
+      </c>
+      <c r="B1" t="str">
+        <v>amount</v>
+      </c>
+      <c r="C1" t="str">
+        <v>date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>i have money</v>
+      </c>
+      <c r="B2">
+        <v>1200</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45828.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>pocket money</v>
+      </c>
+      <c r="B3">
+        <v>5500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45826.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>the mere pe</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45826.22928240741</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>